<commit_message>
added classifications of the sample runs, judgebot still need slight adjustment for the scenario where they agree to a film, and conversation after
</commit_message>
<xml_diff>
--- a/Warehouse/testing/AA/judgement_logs_run4o.xlsx
+++ b/Warehouse/testing/AA/judgement_logs_run4o.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to show "Barbie" on Friday.
+MSG: The decision to acquire the rights for "Barbie" has been successfully recorded.
 </t>
         </is>
       </c>
@@ -478,19 +478,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>./Warehouse/testing/AA/run4o_discovery_04_11_2025 at_16;04;35N.json</t>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_23;42;00N.json</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Barbie" to be shown on Friday.
+MSG: I have determined that there was no decision made regarding the movie to show on Friday. Therefore, I will call the function for no decision.
 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Barbie_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -500,19 +500,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>./Warehouse/testing/AA/run4o_discovery_05_01_2025 at_08;19;27.json</t>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_17_2025 at_23;18;55N.json</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" for the upcoming event.
+MSG: I have recorded the decision as "no decision" regarding which movie to acquire for Friday.
 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>
@@ -522,19 +522,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_23;42;00N.json</t>
+          <t>./Warehouse/testing/AA/run4o_discovery_05_01_2025 at_08;19;27C.json</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for "Oppenheimer" to be shown on Friday.
+MSG: The decision has been made to acquire the rights to both movies.
 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">both_movies, </t>
         </is>
       </c>
     </row>
@@ -544,19 +544,129 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>./Warehouse/testing/AA/run4o_discovery_04_17_2025 at_23;18;55N.json</t>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_23;16;24B.json</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision is to acquire the rights for "Oppenheimer."
+MSG: The decision has been made to acquire the rights for the movie "Barbie."
 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oppenheimer_was_selected, </t>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_23;17;24N.json</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision was made to not reach a conclusion about which movie to show on Friday. Therefore, I have called the function indicating no decision.
+</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_11_2025 at_16;04;35N.json</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: I have recorded the decision that no movie will be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_14;56;36B.json</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded, and the rights to "Barbie" will be acquired for the movie shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Barbie_was_selected, </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_17_2025 at_21;34;16N.json</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: I have recorded the decision as no consensus was reached regarding the movie to be shown on Friday.
+</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>./Warehouse/testing/AA/run4o_discovery_04_24_2025 at_21;27;46N.json</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MSG: None
+MSG: The decision has been recorded as no movie selected for Friday.
+</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">no_decision, </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new classification with latest judge
</commit_message>
<xml_diff>
--- a/Warehouse/testing/AA/judgement_logs_run4o.xlsx
+++ b/Warehouse/testing/AA/judgement_logs_run4o.xlsx
@@ -462,7 +462,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision to acquire the rights for "Barbie" has been successfully recorded.
+MSG: The decision has been recorded, and the rights for "Barbie" will be acquired for Friday's showing.
 </t>
         </is>
       </c>
@@ -484,7 +484,7 @@
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have determined that there was no decision made regarding the movie to show on Friday. Therefore, I will call the function for no decision.
+MSG: The conversation did not result in a decision about which movie to show on Friday.
 </t>
         </is>
       </c>
@@ -506,7 +506,7 @@
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision as "no decision" regarding which movie to acquire for Friday.
+MSG: The decision has been recorded that no movie will be shown on Friday.
 </t>
         </is>
       </c>
@@ -528,7 +528,7 @@
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights to both movies.
+MSG: The rights for both movies, "Oppenheimer" and "Barbie," have been acquired.
 </t>
         </is>
       </c>
@@ -550,7 +550,7 @@
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been made to acquire the rights for the movie "Barbie."
+MSG: The decision has been recorded, and the rights for the movie **"Barbie"** have been acquired.
 </t>
         </is>
       </c>
@@ -572,7 +572,7 @@
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision was made to not reach a conclusion about which movie to show on Friday. Therefore, I have called the function indicating no decision.
+MSG: The decision has been recorded, indicating that no selection for Friday's movie has been made.
 </t>
         </is>
       </c>
@@ -594,7 +594,7 @@
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision that no movie will be shown on Friday.
+MSG: The decision has been recorded as no movie being selected for Friday.
 </t>
         </is>
       </c>
@@ -616,7 +616,7 @@
       <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded, and the rights to "Barbie" will be acquired for the movie shown on Friday.
+MSG: The decision has been made to acquire the rights for "Barbie."
 </t>
         </is>
       </c>
@@ -638,7 +638,7 @@
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: I have recorded the decision as no consensus was reached regarding the movie to be shown on Friday.
+MSG: The decision has been recorded, indicating that no movie was selected for Friday's showing.
 </t>
         </is>
       </c>
@@ -660,7 +660,7 @@
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">MSG: None
-MSG: The decision has been recorded as no movie selected for Friday.
+MSG: The decision has been recorded as no agreement was reached regarding the movie to be shown on Friday.
 </t>
         </is>
       </c>

</xml_diff>